<commit_message>
KARAN: 1) Modified LandingPage, SigninPage and Karan class files 2) Please note the updated name for SigninPage
</commit_message>
<xml_diff>
--- a/Test_Data.xlsx
+++ b/Test_Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\project_kijiji\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C94970C3-4B63-4785-A526-BC294D7AF18C}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{337D52E6-68A6-462C-9822-7F5C21FCE676}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2514,7 +2514,7 @@
   <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Added forgot password testcases
</commit_message>
<xml_diff>
--- a/Test_Data.xlsx
+++ b/Test_Data.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\project_kijiji\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{337D52E6-68A6-462C-9822-7F5C21FCE676}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4505"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Register" sheetId="1" state="hidden" r:id="rId1"/>
@@ -27,8 +21,8 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'sign in'!$A$4:$H$14</definedName>
   </definedNames>
   <calcPr calcId="124519"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -787,8 +781,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1807,7 +1801,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -1859,7 +1853,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -2053,21 +2047,21 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G29"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="13.7109375" customWidth="1"/>
     <col min="2" max="2" width="28.85546875" customWidth="1"/>
@@ -2077,7 +2071,7 @@
     <col min="6" max="6" width="13.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" ht="15.75" thickBot="1">
       <c r="A1" s="1"/>
       <c r="B1" s="84" t="s">
         <v>13</v>
@@ -2088,7 +2082,7 @@
       <c r="F1" s="85"/>
       <c r="G1" s="86"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7">
       <c r="A2" s="1"/>
       <c r="B2" s="78"/>
       <c r="C2" s="79"/>
@@ -2097,7 +2091,7 @@
       <c r="F2" s="79"/>
       <c r="G2" s="80"/>
     </row>
-    <row r="3" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" ht="15.75" thickBot="1">
       <c r="A3" s="1"/>
       <c r="B3" s="81"/>
       <c r="C3" s="82"/>
@@ -2106,7 +2100,7 @@
       <c r="F3" s="82"/>
       <c r="G3" s="83"/>
     </row>
-    <row r="4" spans="1:7" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" ht="34.5" customHeight="1" thickBot="1">
       <c r="A4" s="1" t="s">
         <v>79</v>
       </c>
@@ -2129,7 +2123,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="90">
       <c r="A5" s="1">
         <v>1</v>
       </c>
@@ -2146,7 +2140,7 @@
       <c r="F5" s="9"/>
       <c r="G5" s="11"/>
     </row>
-    <row r="6" spans="1:7" ht="84" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="84" customHeight="1">
       <c r="A6" s="1">
         <v>2</v>
       </c>
@@ -2163,7 +2157,7 @@
       <c r="F6" s="19"/>
       <c r="G6" s="25"/>
     </row>
-    <row r="7" spans="1:7" ht="84" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="84" customHeight="1">
       <c r="A7" s="1">
         <v>3</v>
       </c>
@@ -2180,7 +2174,7 @@
       <c r="F7" s="19"/>
       <c r="G7" s="25"/>
     </row>
-    <row r="8" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" ht="60">
       <c r="A8" s="1">
         <v>4</v>
       </c>
@@ -2197,7 +2191,7 @@
       <c r="F8" s="1"/>
       <c r="G8" s="13"/>
     </row>
-    <row r="9" spans="1:7" ht="70.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="70.5" customHeight="1">
       <c r="A9" s="1">
         <v>5</v>
       </c>
@@ -2214,7 +2208,7 @@
       <c r="F9" s="1"/>
       <c r="G9" s="13"/>
     </row>
-    <row r="10" spans="1:7" ht="70.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" ht="70.5" customHeight="1">
       <c r="A10" s="1">
         <v>6</v>
       </c>
@@ -2231,7 +2225,7 @@
       <c r="F10" s="1"/>
       <c r="G10" s="13"/>
     </row>
-    <row r="11" spans="1:7" ht="70.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" ht="70.5" customHeight="1">
       <c r="A11" s="1">
         <v>7</v>
       </c>
@@ -2248,7 +2242,7 @@
       <c r="F11" s="1"/>
       <c r="G11" s="13"/>
     </row>
-    <row r="12" spans="1:7" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" ht="78.75" customHeight="1">
       <c r="A12" s="1">
         <v>8</v>
       </c>
@@ -2265,7 +2259,7 @@
       <c r="F12" s="1"/>
       <c r="G12" s="13"/>
     </row>
-    <row r="13" spans="1:7" ht="70.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" ht="70.5" customHeight="1">
       <c r="A13" s="1">
         <v>9</v>
       </c>
@@ -2282,7 +2276,7 @@
       <c r="F13" s="1"/>
       <c r="G13" s="13"/>
     </row>
-    <row r="14" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" ht="75">
       <c r="A14" s="1">
         <v>10</v>
       </c>
@@ -2299,7 +2293,7 @@
       <c r="F14" s="1"/>
       <c r="G14" s="13"/>
     </row>
-    <row r="15" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" ht="75">
       <c r="A15" s="1">
         <v>11</v>
       </c>
@@ -2316,7 +2310,7 @@
       <c r="F15" s="1"/>
       <c r="G15" s="13"/>
     </row>
-    <row r="16" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" ht="75">
       <c r="A16" s="1">
         <v>12</v>
       </c>
@@ -2333,7 +2327,7 @@
       <c r="F16" s="1"/>
       <c r="G16" s="13"/>
     </row>
-    <row r="17" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" ht="75">
       <c r="A17" s="1">
         <v>13</v>
       </c>
@@ -2350,7 +2344,7 @@
       <c r="F17" s="1"/>
       <c r="G17" s="13"/>
     </row>
-    <row r="18" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" ht="60">
       <c r="A18" s="1">
         <v>14</v>
       </c>
@@ -2367,7 +2361,7 @@
       <c r="F18" s="1"/>
       <c r="G18" s="13"/>
     </row>
-    <row r="19" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" ht="75">
       <c r="A19" s="1">
         <v>15</v>
       </c>
@@ -2384,7 +2378,7 @@
       <c r="F19" s="1"/>
       <c r="G19" s="13"/>
     </row>
-    <row r="20" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" ht="90">
       <c r="A20" s="1">
         <v>16</v>
       </c>
@@ -2401,7 +2395,7 @@
       <c r="F20" s="1"/>
       <c r="G20" s="13"/>
     </row>
-    <row r="21" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" ht="75">
       <c r="A21" s="1">
         <v>17</v>
       </c>
@@ -2418,7 +2412,7 @@
       <c r="F21" s="1"/>
       <c r="G21" s="13"/>
     </row>
-    <row r="22" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" ht="75">
       <c r="A22" s="1">
         <v>18</v>
       </c>
@@ -2435,7 +2429,7 @@
       <c r="F22" s="1"/>
       <c r="G22" s="13"/>
     </row>
-    <row r="23" spans="1:7" ht="94.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" ht="94.5" customHeight="1">
       <c r="A23" s="1">
         <v>19</v>
       </c>
@@ -2452,7 +2446,7 @@
       <c r="F23" s="1"/>
       <c r="G23" s="13"/>
     </row>
-    <row r="24" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" ht="75">
       <c r="A24" s="1">
         <v>20</v>
       </c>
@@ -2469,7 +2463,7 @@
       <c r="F24" s="1"/>
       <c r="G24" s="13"/>
     </row>
-    <row r="25" spans="1:7" ht="97.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" ht="97.5" customHeight="1">
       <c r="A25" s="1">
         <v>21</v>
       </c>
@@ -2486,16 +2480,16 @@
       <c r="F25" s="1"/>
       <c r="G25" s="1"/>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7">
       <c r="B26" s="37"/>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7">
       <c r="B27" s="37"/>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7">
       <c r="B28" s="37"/>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7">
       <c r="B29" s="37"/>
     </row>
   </sheetData>
@@ -2509,15 +2503,15 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="1"/>
   <dimension ref="A1:H19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="13.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25.5703125" bestFit="1" customWidth="1"/>
@@ -2529,7 +2523,7 @@
     <col min="8" max="8" width="11.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" ht="15.75" thickBot="1">
       <c r="A1" s="4" t="s">
         <v>5</v>
       </c>
@@ -2543,7 +2537,7 @@
       <c r="G1" s="88"/>
       <c r="H1" s="89"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8">
       <c r="A2" s="90" t="s">
         <v>14</v>
       </c>
@@ -2555,7 +2549,7 @@
       <c r="G2" s="91"/>
       <c r="H2" s="92"/>
     </row>
-    <row r="3" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" ht="15.75" thickBot="1">
       <c r="A3" s="93"/>
       <c r="B3" s="94"/>
       <c r="C3" s="94"/>
@@ -2565,7 +2559,7 @@
       <c r="G3" s="94"/>
       <c r="H3" s="95"/>
     </row>
-    <row r="4" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" ht="15.75" thickBot="1">
       <c r="A4" s="21" t="s">
         <v>3</v>
       </c>
@@ -2591,7 +2585,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="91.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="91.5" hidden="1" customHeight="1">
       <c r="A5" s="53">
         <v>1</v>
       </c>
@@ -2611,7 +2605,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="79.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="79.5" hidden="1" customHeight="1">
       <c r="A6" s="26">
         <v>2</v>
       </c>
@@ -2633,7 +2627,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="101.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="101.25" hidden="1" customHeight="1">
       <c r="A7" s="53">
         <v>3</v>
       </c>
@@ -2653,7 +2647,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="101.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="101.25" hidden="1" customHeight="1">
       <c r="A8" s="26">
         <v>4</v>
       </c>
@@ -2673,7 +2667,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="89.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="89.25" hidden="1" customHeight="1">
       <c r="A9" s="53">
         <v>5</v>
       </c>
@@ -2693,7 +2687,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="95.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="95.25" customHeight="1">
       <c r="A10" s="26">
         <v>6</v>
       </c>
@@ -2713,7 +2707,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="90" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" ht="90" hidden="1">
       <c r="A11" s="53">
         <v>7</v>
       </c>
@@ -2733,7 +2727,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="111" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" ht="111" hidden="1" customHeight="1">
       <c r="A12" s="26">
         <v>8</v>
       </c>
@@ -2753,7 +2747,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="86.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" ht="86.25" hidden="1" customHeight="1">
       <c r="A13" s="53">
         <v>9</v>
       </c>
@@ -2773,7 +2767,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="97.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" ht="97.5" hidden="1" customHeight="1" thickBot="1">
       <c r="A14" s="26">
         <v>10</v>
       </c>
@@ -2793,28 +2787,28 @@
         <v>164</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8">
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8">
       <c r="C16" s="3"/>
       <c r="D16" s="3"/>
     </row>
-    <row r="17" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:4">
       <c r="C17" s="3"/>
       <c r="D17" s="3"/>
     </row>
-    <row r="18" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:4">
       <c r="C18" s="3"/>
       <c r="D18" s="3"/>
     </row>
-    <row r="19" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:4">
       <c r="C19" s="3"/>
       <c r="D19" s="3"/>
     </row>
   </sheetData>
-  <autoFilter ref="A4:H14" xr:uid="{4AF4FEED-2CC0-4A74-84CE-E5B498B4EE71}">
+  <autoFilter ref="A4:H14">
     <filterColumn colId="7">
       <filters>
         <filter val="Karan"/>
@@ -2831,15 +2825,15 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="1"/>
   <dimension ref="A1:I18"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="20" customWidth="1"/>
     <col min="2" max="2" width="34.42578125" customWidth="1"/>
@@ -2851,7 +2845,7 @@
     <col min="9" max="9" width="13.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="15.75" thickBot="1">
       <c r="A1" s="18" t="s">
         <v>5</v>
       </c>
@@ -2866,7 +2860,7 @@
       <c r="H1" s="88"/>
       <c r="I1" s="89"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9">
       <c r="A2" s="90" t="s">
         <v>15</v>
       </c>
@@ -2879,7 +2873,7 @@
       <c r="H2" s="91"/>
       <c r="I2" s="92"/>
     </row>
-    <row r="3" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" ht="15.75" thickBot="1">
       <c r="A3" s="93"/>
       <c r="B3" s="94"/>
       <c r="C3" s="94"/>
@@ -2890,7 +2884,7 @@
       <c r="H3" s="94"/>
       <c r="I3" s="95"/>
     </row>
-    <row r="4" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="30">
       <c r="A4" s="5" t="s">
         <v>3</v>
       </c>
@@ -2919,7 +2913,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="352.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" ht="352.5" hidden="1" customHeight="1">
       <c r="A5" s="62">
         <v>1</v>
       </c>
@@ -2942,7 +2936,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="109.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" ht="109.5" customHeight="1">
       <c r="A6" s="63">
         <v>2</v>
       </c>
@@ -2963,7 +2957,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" ht="113.25" hidden="1" customHeight="1">
       <c r="A7" s="63">
         <v>3</v>
       </c>
@@ -2984,7 +2978,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="113.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" ht="113.25" hidden="1" customHeight="1">
       <c r="A8" s="63">
         <v>4</v>
       </c>
@@ -3005,7 +2999,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="125.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" ht="125.25" hidden="1" customHeight="1">
       <c r="A9" s="63">
         <v>5</v>
       </c>
@@ -3026,7 +3020,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="147.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" ht="147.75" hidden="1" customHeight="1">
       <c r="A10" s="63">
         <v>6</v>
       </c>
@@ -3047,7 +3041,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="138.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" ht="138.75" hidden="1" customHeight="1">
       <c r="A11" s="63">
         <v>7</v>
       </c>
@@ -3068,7 +3062,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="201.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" ht="201.75" hidden="1" customHeight="1">
       <c r="A12" s="64">
         <v>8</v>
       </c>
@@ -3089,7 +3083,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="174.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" ht="174.75" hidden="1" customHeight="1">
       <c r="A13" s="63">
         <v>9</v>
       </c>
@@ -3110,7 +3104,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="177.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" ht="177.75" hidden="1" customHeight="1">
       <c r="A14" s="63">
         <v>10</v>
       </c>
@@ -3131,7 +3125,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="285.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" ht="285.75" hidden="1" customHeight="1">
       <c r="A15" s="63">
         <v>11</v>
       </c>
@@ -3152,7 +3146,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="267" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" ht="267" hidden="1" customHeight="1">
       <c r="A16" s="63">
         <v>12</v>
       </c>
@@ -3173,7 +3167,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="259.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" ht="259.5" customHeight="1">
       <c r="A17" s="63">
         <v>13</v>
       </c>
@@ -3194,7 +3188,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="254.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" ht="254.25" hidden="1" customHeight="1" thickBot="1">
       <c r="A18" s="65">
         <v>14</v>
       </c>
@@ -3216,10 +3210,10 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A4:I18" xr:uid="{AD707E63-F036-486D-B861-FFA26FCE24F6}">
+  <autoFilter ref="A4:I18">
     <filterColumn colId="8">
       <filters>
-        <filter val="Karan"/>
+        <filter val="Dipti"/>
       </filters>
     </filterColumn>
   </autoFilter>
@@ -3233,14 +3227,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="15.7109375" customWidth="1"/>
     <col min="2" max="2" width="24.140625" customWidth="1"/>
@@ -3251,7 +3245,7 @@
     <col min="7" max="7" width="42.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" ht="15.75" thickBot="1">
       <c r="A1" s="18" t="s">
         <v>5</v>
       </c>
@@ -3264,7 +3258,7 @@
       <c r="F1" s="96"/>
       <c r="G1" s="97"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7">
       <c r="A2" s="28" t="s">
         <v>148</v>
       </c>
@@ -3275,7 +3269,7 @@
       <c r="F2" s="29"/>
       <c r="G2" s="30"/>
     </row>
-    <row r="3" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" ht="15.75" thickBot="1">
       <c r="A3" s="31"/>
       <c r="B3" s="32"/>
       <c r="C3" s="32"/>
@@ -3284,7 +3278,7 @@
       <c r="F3" s="32"/>
       <c r="G3" s="33"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7">
       <c r="A4" s="5" t="s">
         <v>79</v>
       </c>
@@ -3307,7 +3301,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="168" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="168" customHeight="1">
       <c r="A5" s="1">
         <v>1</v>
       </c>
@@ -3333,34 +3327,34 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="3" width="31.85546875" customWidth="1"/>
     <col min="4" max="5" width="25.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>7</v>
       </c>
@@ -3374,7 +3368,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" s="1" t="s">
         <v>12</v>
       </c>
@@ -3388,7 +3382,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4">
       <c r="A3" s="1" t="s">
         <v>34</v>
       </c>
@@ -3402,7 +3396,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4">
       <c r="A4" s="1" t="s">
         <v>22</v>
       </c>
@@ -3416,7 +3410,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4">
       <c r="A5" s="1" t="s">
         <v>23</v>
       </c>
@@ -3430,7 +3424,7 @@
         <v>11111111</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4">
       <c r="A6" s="1" t="s">
         <v>24</v>
       </c>
@@ -3444,7 +3438,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4">
       <c r="A7" s="1" t="s">
         <v>25</v>
       </c>
@@ -3458,7 +3452,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4">
       <c r="A8" s="1" t="s">
         <v>37</v>
       </c>
@@ -3472,7 +3466,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4">
       <c r="A9" s="1" t="s">
         <v>40</v>
       </c>
@@ -3486,7 +3480,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4">
       <c r="A10" s="1" t="s">
         <v>26</v>
       </c>
@@ -3500,7 +3494,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4">
       <c r="A11" s="1" t="s">
         <v>27</v>
       </c>
@@ -3514,7 +3508,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4">
       <c r="A12" s="1" t="s">
         <v>28</v>
       </c>
@@ -3528,7 +3522,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4">
       <c r="A13" s="1" t="s">
         <v>46</v>
       </c>
@@ -3540,7 +3534,7 @@
       </c>
       <c r="D13" s="1"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4">
       <c r="A14" s="44" t="s">
         <v>42</v>
       </c>
@@ -3552,7 +3546,7 @@
       </c>
       <c r="D14" s="44"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4">
       <c r="A15" s="1" t="s">
         <v>89</v>
       </c>
@@ -3564,7 +3558,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4">
       <c r="A16" s="42" t="s">
         <v>90</v>
       </c>
@@ -3576,7 +3570,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4">
       <c r="A17" s="1" t="s">
         <v>93</v>
       </c>
@@ -3588,7 +3582,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4">
       <c r="A18" s="1" t="s">
         <v>97</v>
       </c>
@@ -3600,7 +3594,7 @@
         <v>11111111</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4">
       <c r="A19" s="44" t="s">
         <v>99</v>
       </c>
@@ -3610,51 +3604,51 @@
       <c r="C19" s="44"/>
       <c r="D19" s="44"/>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4">
       <c r="B20" s="49"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4">
       <c r="B21" s="49"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0500-000000000000}"/>
-    <hyperlink ref="B4" r:id="rId2" xr:uid="{00000000-0004-0000-0500-000001000000}"/>
-    <hyperlink ref="B5" r:id="rId3" xr:uid="{00000000-0004-0000-0500-000002000000}"/>
-    <hyperlink ref="B6" r:id="rId4" xr:uid="{00000000-0004-0000-0500-000003000000}"/>
-    <hyperlink ref="B8" r:id="rId5" xr:uid="{00000000-0004-0000-0500-000004000000}"/>
-    <hyperlink ref="B10" r:id="rId6" xr:uid="{00000000-0004-0000-0500-000005000000}"/>
-    <hyperlink ref="B12" r:id="rId7" xr:uid="{00000000-0004-0000-0500-000006000000}"/>
-    <hyperlink ref="B14" r:id="rId8" xr:uid="{00000000-0004-0000-0500-000007000000}"/>
-    <hyperlink ref="B7" r:id="rId9" xr:uid="{00000000-0004-0000-0500-000008000000}"/>
-    <hyperlink ref="B9" r:id="rId10" xr:uid="{00000000-0004-0000-0500-000009000000}"/>
-    <hyperlink ref="B11" r:id="rId11" xr:uid="{00000000-0004-0000-0500-00000A000000}"/>
-    <hyperlink ref="B13" r:id="rId12" xr:uid="{00000000-0004-0000-0500-00000B000000}"/>
-    <hyperlink ref="B15" r:id="rId13" xr:uid="{00000000-0004-0000-0500-00000C000000}"/>
-    <hyperlink ref="B17" r:id="rId14" xr:uid="{00000000-0004-0000-0500-00000D000000}"/>
-    <hyperlink ref="B18" r:id="rId15" xr:uid="{00000000-0004-0000-0500-00000E000000}"/>
-    <hyperlink ref="B19" r:id="rId16" xr:uid="{00000000-0004-0000-0500-00000F000000}"/>
+    <hyperlink ref="B2" r:id="rId1"/>
+    <hyperlink ref="B4" r:id="rId2"/>
+    <hyperlink ref="B5" r:id="rId3"/>
+    <hyperlink ref="B6" r:id="rId4"/>
+    <hyperlink ref="B8" r:id="rId5"/>
+    <hyperlink ref="B10" r:id="rId6"/>
+    <hyperlink ref="B12" r:id="rId7"/>
+    <hyperlink ref="B14" r:id="rId8"/>
+    <hyperlink ref="B7" r:id="rId9"/>
+    <hyperlink ref="B9" r:id="rId10"/>
+    <hyperlink ref="B11" r:id="rId11"/>
+    <hyperlink ref="B13" r:id="rId12"/>
+    <hyperlink ref="B15" r:id="rId13"/>
+    <hyperlink ref="B17" r:id="rId14"/>
+    <hyperlink ref="B18" r:id="rId15"/>
+    <hyperlink ref="B19" r:id="rId16"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="2" width="25" customWidth="1"/>
     <col min="3" max="3" width="30.5703125" customWidth="1"/>
     <col min="4" max="4" width="20.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>82</v>
       </c>
@@ -3668,7 +3662,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>83</v>
       </c>
@@ -3685,7 +3679,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
         <v>81</v>
       </c>
@@ -3701,28 +3695,28 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" xr:uid="{00000000-0004-0000-0600-000000000000}"/>
-    <hyperlink ref="C3" r:id="rId2" xr:uid="{00000000-0004-0000-0600-000001000000}"/>
+    <hyperlink ref="C2" r:id="rId1"/>
+    <hyperlink ref="C3" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E41D7752-BFC7-4D78-844F-DE2C8E8EC8C7}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="A2" sqref="A2:A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="2" width="9.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="22" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" ht="15.75" thickBot="1">
       <c r="A1" s="76" t="s">
         <v>174</v>
       </c>
@@ -3733,7 +3727,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3">
       <c r="A2" s="98" t="s">
         <v>175</v>
       </c>
@@ -3744,7 +3738,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3">
       <c r="A3" s="99"/>
       <c r="B3" s="72" t="s">
         <v>170</v>
@@ -3753,7 +3747,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3">
       <c r="A4" s="99"/>
       <c r="B4" s="72" t="s">
         <v>166</v>
@@ -3762,7 +3756,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3">
       <c r="A5" s="99"/>
       <c r="B5" s="72" t="s">
         <v>168</v>
@@ -3771,7 +3765,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3">
       <c r="A6" s="99"/>
       <c r="B6" s="72" t="s">
         <v>167</v>
@@ -3780,7 +3774,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3">
       <c r="A7" s="99"/>
       <c r="B7" s="72" t="s">
         <v>165</v>
@@ -3789,7 +3783,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3">
       <c r="A8" s="99"/>
       <c r="B8" s="72" t="s">
         <v>169</v>
@@ -3798,7 +3792,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" ht="15.75" thickBot="1">
       <c r="A9" s="100"/>
       <c r="B9" s="73" t="s">
         <v>171</v>
@@ -3807,7 +3801,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3">
       <c r="A10" s="98" t="s">
         <v>17</v>
       </c>
@@ -3818,7 +3812,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3">
       <c r="A11" s="99"/>
       <c r="B11" s="72" t="s">
         <v>170</v>
@@ -3827,7 +3821,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3">
       <c r="A12" s="99"/>
       <c r="B12" s="72" t="s">
         <v>166</v>
@@ -3836,7 +3830,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3">
       <c r="A13" s="99"/>
       <c r="B13" s="72" t="s">
         <v>168</v>
@@ -3845,7 +3839,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3">
       <c r="A14" s="99"/>
       <c r="B14" s="72" t="s">
         <v>167</v>
@@ -3854,7 +3848,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3">
       <c r="A15" s="99"/>
       <c r="B15" s="72" t="s">
         <v>165</v>
@@ -3863,7 +3857,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3">
       <c r="A16" s="99"/>
       <c r="B16" s="72" t="s">
         <v>169</v>
@@ -3872,7 +3866,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" ht="15.75" thickBot="1">
       <c r="A17" s="99"/>
       <c r="B17" s="74" t="s">
         <v>171</v>
@@ -3881,7 +3875,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" ht="15.75" thickBot="1">
       <c r="A18" s="21" t="s">
         <v>176</v>
       </c>

</xml_diff>